<commit_message>
update errors and RL
</commit_message>
<xml_diff>
--- a/exp4/exp4.xlsx
+++ b/exp4/exp4.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7542" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="2" r:id="rId1"/>
     <sheet name="RC" sheetId="1" r:id="rId2"/>
     <sheet name="RL" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="68">
   <si>
     <t>R [ohm]</t>
   </si>
@@ -218,6 +218,9 @@
   <si>
     <t xml:space="preserve">eta13 = </t>
   </si>
+  <si>
+    <t>dR</t>
+  </si>
 </sst>
 </file>
 
@@ -302,6 +305,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -679,6 +683,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1056,6 +1061,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1270,6 +1276,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>f^2 [Hz^2]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1332,6 +1394,77 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>|Z|^2 [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Ω</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>^2]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1433,6 +1566,49 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>tan(</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="el-GR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>φ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1647,6 +1823,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>f</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> [Hz]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1709,6 +1946,77 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>tan(</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>φ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4225,23 +4533,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4277,23 +4568,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4472,21 +4746,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.36328125" customWidth="1"/>
-    <col min="9" max="9" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.3671875" customWidth="1"/>
+    <col min="9" max="9" width="13.89453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.26953125" customWidth="1"/>
-    <col min="13" max="13" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.26171875" customWidth="1"/>
+    <col min="13" max="13" width="13.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4512,7 +4786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>220</v>
       </c>
@@ -4538,7 +4812,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="G4" t="s">
         <v>29</v>
       </c>
@@ -4554,7 +4828,7 @@
         <v>4.090909090909091E-8</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="G5" t="s">
         <v>31</v>
       </c>
@@ -4570,11 +4844,12 @@
         <v>24444444.444444444</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="G8" t="s">
         <v>57</v>
       </c>
       <c r="H8">
+        <f>'RC'!X32</f>
         <v>2.2902282688310729E-6</v>
       </c>
       <c r="I8" t="s">
@@ -4584,31 +4859,35 @@
         <v>60</v>
       </c>
       <c r="L8">
+        <f>RL!AG9</f>
         <v>1.75021537170548E-2</v>
       </c>
       <c r="M8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="G9" t="s">
         <v>50</v>
       </c>
       <c r="H9">
+        <f>'RC'!X33</f>
         <v>2.3783026063257521E-7</v>
       </c>
       <c r="K9" t="s">
         <v>51</v>
       </c>
       <c r="L9">
+        <f>RL!AG10</f>
         <v>1.1639432906807199E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="G11" t="s">
         <v>58</v>
       </c>
       <c r="H11">
+        <f>'RC'!W7</f>
         <v>2.3364373181542564E-6</v>
       </c>
       <c r="I11" t="s">
@@ -4618,43 +4897,46 @@
         <v>61</v>
       </c>
       <c r="L11">
+        <f>RL!AD34</f>
         <v>7.2762688408420069E-3</v>
       </c>
       <c r="M11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="G12" t="s">
         <v>50</v>
       </c>
       <c r="H12">
-        <v>4.7866331241200509E-8</v>
+        <f>'RC'!W8</f>
+        <v>4.8159969551735215E-8</v>
       </c>
       <c r="K12" t="s">
         <v>51</v>
       </c>
       <c r="L12">
-        <v>9.8076304224935256E-5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+        <f>RL!AD35</f>
+        <v>9.9460710738507585E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="G14" s="3" t="s">
         <v>62</v>
       </c>
       <c r="H14" s="3">
         <f>(ABS(H11-H8)/(SQRT(H9^2+H12^2)))</f>
-        <v>0.19047478718292762</v>
+        <v>0.19042917558095881</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>62</v>
       </c>
       <c r="L14" s="2">
         <f>ABS(L8-L11)/(SQRT(L9^2+L12^2))</f>
-        <v>8.7545284423926564</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+        <v>8.7536512127053019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="G15" s="3" t="s">
         <v>63</v>
       </c>
@@ -4670,20 +4952,20 @@
         <v>7.2978812145216612</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="G16" s="3" t="s">
         <v>64</v>
       </c>
       <c r="H16" s="3">
         <f>(ABS(G2-H11)/SQRT(H12^2+H2^2))</f>
-        <v>6.9906486908587242</v>
+        <v>6.9484815949691541</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>66</v>
       </c>
       <c r="L16" s="4">
         <f>ABS(K2-L11)/SQRT(L12^2+L2^2)</f>
-        <v>15.658019523863427</v>
+        <v>15.484288086757632</v>
       </c>
     </row>
   </sheetData>
@@ -4696,23 +4978,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y52"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7:W8"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="23" max="24" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="11.7890625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.7890625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.89453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -4735,7 +5017,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="G3" t="s">
         <v>18</v>
       </c>
@@ -4757,7 +5039,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -4806,7 +5088,7 @@
         <v>3.2296590982860383E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>0</v>
       </c>
@@ -4834,11 +5116,18 @@
         <f>P23</f>
         <v>2.2655969134909779</v>
       </c>
+      <c r="U5" t="s">
+        <v>67</v>
+      </c>
+      <c r="V5">
+        <f>Values!B2</f>
+        <v>0.5</v>
+      </c>
       <c r="X5">
         <v>6.6165666415926499E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -4876,7 +5165,7 @@
         <v>2.5181301766758906</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -4904,7 +5193,7 @@
         <v>2.3364373181542564E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="R8">
         <v>300</v>
       </c>
@@ -4916,17 +5205,17 @@
         <v>50</v>
       </c>
       <c r="W8">
-        <f>X5/(2*PI()*V4)</f>
-        <v>4.7866331241200509E-8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+        <f>SQRT(POWER(X5/(2*PI()*V4),2)+POWER(V5*X4/(2*PI()*V4*V4),2))</f>
+        <v>4.8159969551735215E-8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>23</v>
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -4940,7 +5229,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="G12" t="s">
         <v>18</v>
       </c>
@@ -4949,7 +5238,7 @@
         <v>0.50460526315789478</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -4981,7 +5270,7 @@
         <v>1.8059572291935382</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>0</v>
       </c>
@@ -5003,7 +5292,7 @@
         <v>1.9140494383701192</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -5034,7 +5323,7 @@
         <v>2.0221416475467002</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -5048,13 +5337,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -5068,7 +5357,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="G21" t="s">
         <v>18</v>
       </c>
@@ -5077,7 +5366,7 @@
         <v>0.44683544303797462</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -5109,7 +5398,7 @@
         <v>2.2208585375639172</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>0</v>
       </c>
@@ -5131,7 +5420,7 @@
         <v>2.2655969134909779</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -5162,7 +5451,7 @@
         <v>2.3103352894180387</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -5188,7 +5477,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="R26">
         <v>500</v>
       </c>
@@ -5205,7 +5494,7 @@
         <v>7.3514389676004207E-5</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="R27">
         <v>600</v>
       </c>
@@ -5222,7 +5511,7 @@
         <v>9.8604154827806547E-5</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -5243,7 +5532,7 @@
         <v>1.2353667252207318E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -5276,7 +5565,7 @@
         <v>2.0707004536655458E-10</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="G30" t="s">
         <v>18</v>
       </c>
@@ -5303,7 +5592,7 @@
         <v>2.2330269283953883E-12</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -5350,7 +5639,7 @@
         <v>4.0543259663300723E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>0</v>
       </c>
@@ -5379,7 +5668,7 @@
         <v>2.2902282688310729E-6</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -5417,7 +5706,7 @@
         <v>2.3783026063257521E-7</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -5431,13 +5720,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>26</v>
       </c>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -5451,7 +5740,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="G39" t="s">
         <v>18</v>
       </c>
@@ -5460,7 +5749,7 @@
         <v>0.66962962962962957</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -5492,7 +5781,7 @@
         <v>1.2369420621348701</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>0</v>
       </c>
@@ -5514,7 +5803,7 @@
         <v>1.2466413544959245</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -5545,7 +5834,7 @@
         <v>1.2563406468569787</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -5559,13 +5848,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>27</v>
       </c>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -5579,7 +5868,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="G48" t="s">
         <v>18</v>
       </c>
@@ -5588,7 +5877,7 @@
         <v>0.79032258064516125</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -5620,7 +5909,7 @@
         <v>0.90979819830745656</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>0</v>
       </c>
@@ -5642,7 +5931,7 @@
         <v>0.93896292376760759</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -5673,7 +5962,7 @@
         <v>0.96812764922775862</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -5697,18 +5986,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH52"/>
   <sheetViews>
-    <sheetView topLeftCell="Y20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AC34" sqref="AC34:AD35"/>
+    <sheetView topLeftCell="U1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="11" width="0" hidden="1" customWidth="1"/>
     <col min="30" max="31" width="12" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -5716,7 +6005,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -5759,7 +6048,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="S3" s="1"/>
       <c r="Y3">
         <v>4100</v>
@@ -5781,7 +6070,7 @@
         <v>468932.43429775722</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -5844,7 +6133,7 @@
         <v>425670.01616840443</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>0</v>
       </c>
@@ -5906,7 +6195,7 @@
         <v>579890.63086519588</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -5975,7 +6264,7 @@
         <v>1.2093241461400176E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -6043,7 +6332,7 @@
         <v>5.3483938312562898E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="Y8">
         <v>9300</v>
       </c>
@@ -6064,7 +6353,7 @@
         <v>1309938.3223950451</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="AF9" t="s">
         <v>46</v>
       </c>
@@ -6073,7 +6362,7 @@
         <v>1.75021537170548E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -6094,7 +6383,7 @@
         <v>1.1639432906807199E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -6122,7 +6411,7 @@
       </c>
       <c r="R11" s="1"/>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -6165,7 +6454,7 @@
         <v>3.346228239845261</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>0</v>
       </c>
@@ -6208,7 +6497,7 @@
         <v>0.5826589595375723</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -6254,7 +6543,7 @@
         <v>3.1135135135135137</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -6300,12 +6589,12 @@
         <v>0.62620889748549313</v>
       </c>
     </row>
-    <row r="19" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="19" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="20" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L20" t="s">
         <v>6</v>
       </c>
@@ -6320,7 +6609,7 @@
       </c>
       <c r="R20" s="1"/>
     </row>
-    <row r="22" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="22" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L22" t="s">
         <v>8</v>
       </c>
@@ -6344,7 +6633,7 @@
         <v>3.8235294117647061</v>
       </c>
     </row>
-    <row r="23" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="23" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L23">
         <v>0</v>
       </c>
@@ -6368,7 +6657,7 @@
         <v>0.71208791208791211</v>
       </c>
     </row>
-    <row r="24" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="24" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L24" t="s">
         <v>7</v>
       </c>
@@ -6392,7 +6681,7 @@
         <v>3.7161290322580647</v>
       </c>
     </row>
-    <row r="25" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="25" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L25" t="s">
         <v>9</v>
       </c>
@@ -6416,7 +6705,7 @@
         <v>0.73266806722689082</v>
       </c>
     </row>
-    <row r="28" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="28" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L28" t="s">
         <v>35</v>
       </c>
@@ -6427,7 +6716,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="29" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L29" t="s">
         <v>6</v>
       </c>
@@ -6449,7 +6738,7 @@
         <v>0.83665035106532015</v>
       </c>
     </row>
-    <row r="30" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="30" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="Y30">
         <v>3700</v>
       </c>
@@ -6458,7 +6747,7 @@
         <v>0.75871452560888286</v>
       </c>
     </row>
-    <row r="31" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="31" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L31" t="s">
         <v>8</v>
       </c>
@@ -6489,7 +6778,7 @@
         <v>1.0446560505420173</v>
       </c>
     </row>
-    <row r="32" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="32" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L32">
         <v>0</v>
       </c>
@@ -6523,6 +6812,7 @@
         <v>47</v>
       </c>
       <c r="AC32">
+        <f>Values!A2</f>
         <v>220</v>
       </c>
       <c r="AE32">
@@ -6530,7 +6820,7 @@
         <v>2.0780975214485062E-4</v>
       </c>
     </row>
-    <row r="33" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="33" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L33" t="s">
         <v>7</v>
       </c>
@@ -6560,11 +6850,18 @@
         <f>TAN(ASIN((W41+W43)/2))</f>
         <v>1.5022350267712594</v>
       </c>
+      <c r="AB33" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC33">
+        <f>Values!B2</f>
+        <v>0.5</v>
+      </c>
       <c r="AE33">
         <v>2.8010526985844929E-6</v>
       </c>
     </row>
-    <row r="34" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="34" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L34" t="s">
         <v>9</v>
       </c>
@@ -6602,21 +6899,21 @@
         <v>7.2762688408420069E-3</v>
       </c>
     </row>
-    <row r="35" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="35" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="AC35" t="s">
         <v>51</v>
       </c>
       <c r="AD35">
-        <f>(AE33*AC32/(2*PI()))</f>
-        <v>9.8076304224935256E-5</v>
-      </c>
-    </row>
-    <row r="37" spans="12:31" x14ac:dyDescent="0.35">
+        <f>SQRT(POWER((AE33*AC32/(2*PI())),2)+POWER((AE32*AC33/(2*PI())),2))</f>
+        <v>9.9460710738507585E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="38" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L38" t="s">
         <v>6</v>
       </c>
@@ -6631,7 +6928,7 @@
       </c>
       <c r="R38" s="1"/>
     </row>
-    <row r="40" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="40" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L40" t="s">
         <v>8</v>
       </c>
@@ -6655,7 +6952,7 @@
         <v>4.7911547911547911</v>
       </c>
     </row>
-    <row r="41" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="41" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L41">
         <v>0</v>
       </c>
@@ -6679,7 +6976,7 @@
         <v>0.82641025641025645</v>
       </c>
     </row>
-    <row r="42" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="42" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L42" t="s">
         <v>7</v>
       </c>
@@ -6703,7 +7000,7 @@
         <v>4.7223443223443224</v>
       </c>
     </row>
-    <row r="43" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="43" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L43" t="s">
         <v>9</v>
       </c>
@@ -6727,12 +7024,12 @@
         <v>0.83845208845208852</v>
       </c>
     </row>
-    <row r="46" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="46" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L46" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="12:31" x14ac:dyDescent="0.35">
+    <row r="47" spans="12:31" x14ac:dyDescent="0.55000000000000004">
       <c r="L47" t="s">
         <v>6</v>
       </c>
@@ -6747,7 +7044,7 @@
       </c>
       <c r="R47" s="1"/>
     </row>
-    <row r="49" spans="12:23" x14ac:dyDescent="0.35">
+    <row r="49" spans="12:23" x14ac:dyDescent="0.55000000000000004">
       <c r="L49" t="s">
         <v>8</v>
       </c>
@@ -6771,7 +7068,7 @@
         <v>5.6779661016949152</v>
       </c>
     </row>
-    <row r="50" spans="12:23" x14ac:dyDescent="0.35">
+    <row r="50" spans="12:23" x14ac:dyDescent="0.55000000000000004">
       <c r="L50">
         <v>0</v>
       </c>
@@ -6795,7 +7092,7 @@
         <v>0.8860696517412936</v>
       </c>
     </row>
-    <row r="51" spans="12:23" x14ac:dyDescent="0.35">
+    <row r="51" spans="12:23" x14ac:dyDescent="0.55000000000000004">
       <c r="L51" t="s">
         <v>7</v>
       </c>
@@ -6819,7 +7116,7 @@
         <v>5.6539682539682534</v>
       </c>
     </row>
-    <row r="52" spans="12:23" x14ac:dyDescent="0.35">
+    <row r="52" spans="12:23" x14ac:dyDescent="0.55000000000000004">
       <c r="L52" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
data analysis & report update
</commit_message>
<xml_diff>
--- a/exp4/exp4.xlsx
+++ b/exp4/exp4.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="68">
   <si>
     <t>R [ohm]</t>
   </si>
@@ -5074,13 +5074,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.3671875" customWidth="1"/>
@@ -5174,7 +5174,7 @@
         <v>24444444.444444444</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="G8" t="s">
         <v>57</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="G9" t="s">
         <v>50</v>
       </c>
@@ -5212,7 +5212,8 @@
         <v>1.1639432906807199E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="11" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="G11" t="s">
         <v>58</v>
       </c>
@@ -5234,7 +5235,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="G12" t="s">
         <v>50</v>
       </c>
@@ -5250,7 +5251,8 @@
         <v>9.9460710738507585E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="14" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="G14" s="3" t="s">
         <v>62</v>
       </c>
@@ -5266,7 +5268,7 @@
         <v>8.7536512127053019</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="G15" s="3" t="s">
         <v>63</v>
       </c>
@@ -5282,7 +5284,7 @@
         <v>6.9080658285574943</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="G16" s="3" t="s">
         <v>64</v>
       </c>
@@ -5296,6 +5298,125 @@
       <c r="L16" s="4">
         <f>ABS(K2-L11)/SQRT(L12^2+L2^2)</f>
         <v>4.1819854198940103</v>
+      </c>
+    </row>
+    <row r="17" spans="7:13" collapsed="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="20" spans="7:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="G20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2.3E-6</v>
+      </c>
+      <c r="I20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K20" t="s">
+        <v>60</v>
+      </c>
+      <c r="L20" s="1">
+        <f>0.017</f>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="M20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="7:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="G21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" s="1">
+        <v>2.4999999999999999E-7</v>
+      </c>
+      <c r="K21" t="s">
+        <v>51</v>
+      </c>
+      <c r="L21" s="1">
+        <f>0.001</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="7:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="G23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="1">
+        <v>2.34E-6</v>
+      </c>
+      <c r="I23" t="s">
+        <v>55</v>
+      </c>
+      <c r="K23" t="s">
+        <v>61</v>
+      </c>
+      <c r="L23" s="1">
+        <v>7.9000000000000008E-3</v>
+      </c>
+      <c r="M23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="7:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="G24" t="s">
+        <v>50</v>
+      </c>
+      <c r="H24" s="1">
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="K24" t="s">
+        <v>51</v>
+      </c>
+      <c r="L24" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="7:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="G26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H26" s="3">
+        <f>(ABS(H23-H20)/(SQRT(H21^2+H24^2)))</f>
+        <v>7.1554175279993346E-2</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L26" s="2">
+        <f>ABS(L20-L23)/(SQRT(L21^2+L24^2))</f>
+        <v>9.0548384309109018</v>
+      </c>
+    </row>
+    <row r="27" spans="7:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="G27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" s="3">
+        <f>(ABS(G2-H20)/SQRT(H21^2+H2^2))</f>
+        <v>1.1961783342433503</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L27" s="4">
+        <f>ABS(K2-L20)/SQRT(L21^2+L2^2)</f>
+        <v>7.4278135270820771</v>
+      </c>
+    </row>
+    <row r="28" spans="7:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="G28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" s="3">
+        <f>(ABS(G2-H23)/SQRT(H24^2+H2^2))</f>
+        <v>0.67945665193081717</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L28" s="4">
+        <f>ABS(K2-L23)/SQRT(L24^2+L2^2)</f>
+        <v>2.667891875399659</v>
       </c>
     </row>
   </sheetData>
@@ -5308,8 +5429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView topLeftCell="R4" workbookViewId="0">
-      <selection activeCell="Z29" sqref="Z29"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5501,6 +5622,7 @@
         <f>P32*-1</f>
         <v>-2.5181301766758906</v>
       </c>
+      <c r="X6" s="1"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
@@ -6329,8 +6451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI52"/>
   <sheetViews>
-    <sheetView topLeftCell="AB19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AE33" sqref="AE33"/>
+    <sheetView topLeftCell="AA10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AD35" sqref="AD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6707,7 +6829,7 @@
         <v>46</v>
       </c>
       <c r="AG9">
-        <f>SQRT(AH6/(4*PI()^2))</f>
+        <f>SQRT(AH6/(4*PI()*PI()))</f>
         <v>1.75021537170548E-2</v>
       </c>
     </row>

</xml_diff>